<commit_message>
Enables practice trials list gen | minor fixes
fix trials gen to enable practice gen
Added max cap length
Added new trial lists
fixed tests.m
added failed tests log
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/word_lists/art_primes.xlsx
+++ b/experiment/RUN_ME/stimuli/word_lists/art_primes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\stimuli\word_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\word_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FECA62-ED73-4226-9FB4-FC82DFAF4A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{563CDB29-4F43-4342-87F6-E7D41F73E2A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{45E0E9EB-DD48-4B7C-811F-EF25922830D0}"/>
+    <workbookView xWindow="3930" yWindow="3930" windowWidth="18900" windowHeight="11055" xr2:uid="{45E0E9EB-DD48-4B7C-811F-EF25922830D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="30">
   <si>
     <t>אגרטל</t>
   </si>
@@ -101,9 +101,6 @@
     <t>גיטרה</t>
   </si>
   <si>
-    <t>גלידה</t>
-  </si>
-  <si>
     <t>ספינה</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>תמרור</t>
+  </si>
+  <si>
+    <t>צוללת</t>
   </si>
 </sst>
 </file>
@@ -500,14 +500,16 @@
     <col min="3" max="4" width="6.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.25" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="6.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.75" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="6.375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="5.75" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="6.625" bestFit="1" customWidth="1"/>
   </cols>
@@ -523,13 +525,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -544,7 +546,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -562,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
@@ -586,22 +588,22 @@
         <v>19</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -807,55 +809,52 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -904,9 +903,6 @@
       <c r="Z6" t="s">
         <v>3</v>
       </c>
-      <c r="AA6" t="s">
-        <v>3</v>
-      </c>
       <c r="AB6" t="s">
         <v>3</v>
       </c>
@@ -919,61 +915,61 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Z7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AD7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -1028,6 +1024,9 @@
       <c r="W8" t="s">
         <v>4</v>
       </c>
+      <c r="AA8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1196,6 +1195,9 @@
       <c r="Z11" t="s">
         <v>7</v>
       </c>
+      <c r="AA11" t="s">
+        <v>7</v>
+      </c>
       <c r="AB11" t="s">
         <v>7</v>
       </c>
@@ -1208,61 +1210,61 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -1308,9 +1310,6 @@
       <c r="Z13" t="s">
         <v>8</v>
       </c>
-      <c r="AA13" t="s">
-        <v>8</v>
-      </c>
       <c r="AC13" t="s">
         <v>8</v>
       </c>
@@ -1364,6 +1363,9 @@
       <c r="W14" t="s">
         <v>9</v>
       </c>
+      <c r="AA14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1420,9 +1422,6 @@
       <c r="Z15" t="s">
         <v>10</v>
       </c>
-      <c r="AA15" t="s">
-        <v>10</v>
-      </c>
       <c r="AB15" t="s">
         <v>10</v>
       </c>
@@ -1479,6 +1478,9 @@
       <c r="W16" t="s">
         <v>11</v>
       </c>
+      <c r="AA16" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1538,9 +1540,6 @@
       <c r="Y17" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" t="s">
-        <v>12</v>
-      </c>
       <c r="AC17" t="s">
         <v>12</v>
       </c>
@@ -1550,67 +1549,67 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AA18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AB18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AC18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AD18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -1724,6 +1723,9 @@
       <c r="Y20" t="s">
         <v>14</v>
       </c>
+      <c r="AA20" t="s">
+        <v>14</v>
+      </c>
       <c r="AC20" t="s">
         <v>14</v>
       </c>
@@ -1827,6 +1829,9 @@
       <c r="W22" t="s">
         <v>16</v>
       </c>
+      <c r="AA22" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1883,6 +1888,9 @@
       <c r="Z23" t="s">
         <v>17</v>
       </c>
+      <c r="AA23" t="s">
+        <v>17</v>
+      </c>
       <c r="AB23" t="s">
         <v>17</v>
       </c>
@@ -1945,9 +1953,6 @@
       <c r="Z24" t="s">
         <v>18</v>
       </c>
-      <c r="AA24" t="s">
-        <v>18</v>
-      </c>
       <c r="AB24" t="s">
         <v>18</v>
       </c>
@@ -2001,40 +2006,40 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -2086,196 +2091,223 @@
       <c r="W27" t="s">
         <v>20</v>
       </c>
+      <c r="AA27" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="J28" t="s">
+        <v>29</v>
       </c>
       <c r="K28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" t="s">
-        <v>21</v>
-      </c>
-      <c r="N28" t="s">
-        <v>21</v>
-      </c>
-      <c r="P28" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" t="s">
+        <v>29</v>
       </c>
       <c r="Q28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="R28" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="S28" t="s">
+        <v>29</v>
       </c>
       <c r="T28" t="s">
-        <v>21</v>
-      </c>
-      <c r="W28" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="U28" t="s">
+        <v>29</v>
+      </c>
+      <c r="V28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W29" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W30" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W31" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>